<commit_message>
Updates to process the latest ERSD JSON file.
</commit_message>
<xml_diff>
--- a/documents/eCR_R1.1_FHIR_Mapping_R4.xlsx
+++ b/documents/eCR_R1.1_FHIR_Mapping_R4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbashyam/git/eCRNow/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3C38C3-E78E-1542-9F0D-22CBE205F520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C874D46-65A2-4449-8910-8E283ABE1073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="1400" windowWidth="33420" windowHeight="17640" activeTab="1" xr2:uid="{0236C1A8-3996-47BC-AEF5-83819174BBEE}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Loading Queries" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Loading Queries'!$A$1:$S$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Loading Queries'!$A$1:$T$102</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="429">
   <si>
     <t>Data Element</t>
   </si>
@@ -1399,9 +1399,6 @@
   </si>
   <si>
     <t>Implemented</t>
-  </si>
-  <si>
-    <t>Implemented (Version Number Incrementer not tested)</t>
   </si>
   <si>
     <t>Not tested</t>
@@ -2034,7 +2031,7 @@
         <v>423</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -2105,10 +2102,10 @@
   <dimension ref="A1:T102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T46" sqref="T46"/>
+      <selection pane="bottomRight" activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2131,7 +2128,7 @@
     <col min="16" max="16" width="71.6640625" style="30" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="24.6640625" style="31" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="78" style="31" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="57.83203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.83203125" style="32" customWidth="1"/>
     <col min="20" max="20" width="26.5" style="32" customWidth="1"/>
     <col min="21" max="16384" width="9.1640625" style="25"/>
   </cols>
@@ -2366,7 +2363,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>107</v>
       </c>
@@ -2419,7 +2416,7 @@
       </c>
       <c r="S5" s="9"/>
       <c r="T5" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.15">
@@ -2683,7 +2680,7 @@
       <c r="R10" s="10"/>
       <c r="S10" s="9"/>
       <c r="T10" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.15">
@@ -2733,7 +2730,7 @@
       <c r="R11" s="10"/>
       <c r="S11" s="9"/>
       <c r="T11" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:20" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.15">
@@ -2783,7 +2780,7 @@
       <c r="R12" s="10"/>
       <c r="S12" s="9"/>
       <c r="T12" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.15">
@@ -4127,7 +4124,7 @@
         <v>389</v>
       </c>
       <c r="T39" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="40" spans="1:20" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.15">
@@ -4179,7 +4176,7 @@
       <c r="R40" s="9"/>
       <c r="S40" s="9"/>
       <c r="T40" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="41" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4475,7 +4472,7 @@
         <v>391</v>
       </c>
       <c r="T46" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="47" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4527,7 +4524,7 @@
       </c>
       <c r="S47" s="9"/>
       <c r="T47" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="48" spans="1:20" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
@@ -4579,7 +4576,7 @@
       </c>
       <c r="S48" s="9"/>
       <c r="T48" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="49" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4629,7 +4626,7 @@
       <c r="R49" s="9"/>
       <c r="S49" s="9"/>
       <c r="T49" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="50" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4679,7 +4676,7 @@
       <c r="R50" s="9"/>
       <c r="S50" s="9"/>
       <c r="T50" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="51" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4729,7 +4726,7 @@
       <c r="R51" s="9"/>
       <c r="S51" s="9"/>
       <c r="T51" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="52" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4773,7 +4770,7 @@
       <c r="R52" s="5"/>
       <c r="S52" s="9"/>
       <c r="T52" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="53" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4819,7 +4816,7 @@
       </c>
       <c r="S53" s="9"/>
       <c r="T53" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="54" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -4865,7 +4862,7 @@
       </c>
       <c r="S54" s="9"/>
       <c r="T54" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="55" spans="1:20" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.15">
@@ -5815,7 +5812,7 @@
       <c r="R72" s="9"/>
       <c r="S72" s="9"/>
       <c r="T72" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="73" spans="1:20" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
@@ -5865,7 +5862,7 @@
       <c r="R73" s="9"/>
       <c r="S73" s="9"/>
       <c r="T73" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="74" spans="1:20" s="4" customFormat="1" ht="78" x14ac:dyDescent="0.15">
@@ -5981,7 +5978,7 @@
         <v>121</v>
       </c>
       <c r="T75" s="9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="76" spans="1:20" s="4" customFormat="1" ht="52" x14ac:dyDescent="0.15">
@@ -6331,7 +6328,7 @@
         <v>406</v>
       </c>
       <c r="T83" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="84" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -6379,7 +6376,7 @@
       </c>
       <c r="S84" s="29"/>
       <c r="T84" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="85" spans="1:20" ht="65" x14ac:dyDescent="0.15">
@@ -6429,7 +6426,7 @@
       <c r="R85" s="29"/>
       <c r="S85" s="29"/>
       <c r="T85" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="86" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -6475,7 +6472,7 @@
       <c r="R86" s="29"/>
       <c r="S86" s="29"/>
       <c r="T86" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="87" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -6521,7 +6518,7 @@
       <c r="R87" s="29"/>
       <c r="S87" s="29"/>
       <c r="T87" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="88" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -6567,7 +6564,7 @@
       <c r="R88" s="29"/>
       <c r="S88" s="29"/>
       <c r="T88" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="89" spans="1:20" ht="13" x14ac:dyDescent="0.15">
@@ -6613,7 +6610,7 @@
       <c r="R89" s="29"/>
       <c r="S89" s="29"/>
       <c r="T89" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="90" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -7145,7 +7142,7 @@
         <v>407</v>
       </c>
       <c r="T99" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="100" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -7179,7 +7176,7 @@
       <c r="R100" s="9"/>
       <c r="S100" s="9"/>
       <c r="T100" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="101" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -7213,7 +7210,7 @@
       <c r="R101" s="9"/>
       <c r="S101" s="9"/>
       <c r="T101" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="102" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -7247,17 +7244,39 @@
       <c r="R102" s="9"/>
       <c r="S102" s="9"/>
       <c r="T102" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S102" xr:uid="{7FA853B4-9A4E-4B12-8E65-2E02242B8B58}"/>
+  <autoFilter ref="A1:T102" xr:uid="{AD5EB5E7-6303-FD4B-B523-8263850D5D08}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </LCG_x0020_Document_x0020_Workflow>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AAEF04E9A1B48544A813770D804417BF" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5f6564d6fd1be9d83e2a64915f5205a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9ed5a28f-e285-4793-933e-f86572ea3e88" xmlns:ns3="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628" xmlns:ns4="a130c0bc-081d-4a7d-8c4b-0d956631a56e" xmlns:ns5="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e84ddf88720b63dcc3a8c6c9e2ce95b4" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7508,29 +7527,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF9989B-4098-42D7-BF53-B78163861EAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </LCG_x0020_Document_x0020_Workflow>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F38DC35-61B7-4F0C-AF24-8F7D63AD6B02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7550,23 +7566,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF9989B-4098-42D7-BF53-B78163861EAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Formatting and Name Updates and Unit Test Fixe.
</commit_message>
<xml_diff>
--- a/documents/eCR_R1.1_FHIR_Mapping_R4.xlsx
+++ b/documents/eCR_R1.1_FHIR_Mapping_R4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbashyam/git/eCRNow/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C874D46-65A2-4449-8910-8E283ABE1073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF20E96E-6263-7442-A123-5E3C372EBF4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="1400" windowWidth="33420" windowHeight="17640" activeTab="1" xr2:uid="{0236C1A8-3996-47BC-AEF5-83819174BBEE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="431">
   <si>
     <t>Data Element</t>
   </si>
@@ -1406,6 +1406,13 @@
   <si>
     <t xml:space="preserve">Implemented
 </t>
+  </si>
+  <si>
+    <t>DiagnosticReport.code or Observation.code when DiagnosticReport is not available.</t>
+  </si>
+  <si>
+    <t>Encounter.participant.individual.Practitioner (Use ATTENDING PHYSICIAN first, if not use Admitting Physician, If that is not there then use a Software System as the author)
+Condition.asserter.Practitioner</t>
   </si>
 </sst>
 </file>
@@ -2102,10 +2109,10 @@
   <dimension ref="A1:T102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T6" sqref="T6"/>
+      <selection pane="bottomRight" activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -3319,7 +3326,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:20" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
         <v>156</v>
       </c>
@@ -3945,7 +3952,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
         <v>167</v>
       </c>
@@ -3974,8 +3981,8 @@
       <c r="L36" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="M36" s="8" t="s">
-        <v>371</v>
+      <c r="M36" s="11" t="s">
+        <v>430</v>
       </c>
       <c r="N36" s="8"/>
       <c r="O36" s="8" t="s">
@@ -4901,7 +4908,7 @@
         <v>341</v>
       </c>
       <c r="M55" s="8" t="s">
-        <v>336</v>
+        <v>429</v>
       </c>
       <c r="N55" s="13" t="s">
         <v>92</v>
@@ -7255,28 +7262,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </LCG_x0020_Document_x0020_Workflow>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AAEF04E9A1B48544A813770D804417BF" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5f6564d6fd1be9d83e2a64915f5205a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9ed5a28f-e285-4793-933e-f86572ea3e88" xmlns:ns3="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628" xmlns:ns4="a130c0bc-081d-4a7d-8c4b-0d956631a56e" xmlns:ns5="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e84ddf88720b63dcc3a8c6c9e2ce95b4" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7527,26 +7512,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF9989B-4098-42D7-BF53-B78163861EAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </LCG_x0020_Document_x0020_Workflow>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F38DC35-61B7-4F0C-AF24-8F7D63AD6B02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7566,4 +7554,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECF9989B-4098-42D7-BF53-B78163861EAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>